<commit_message>
Adjusting study cases and adding evidences for the bugs resolved
</commit_message>
<xml_diff>
--- a/Testing/Testing Manual/INTEGRADOR DH TESTING.xlsx
+++ b/Testing/Testing Manual/INTEGRADOR DH TESTING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DeveloperTraining\ProyectoIntegradorG7\grupo-07\Testing\Testing Manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C588386-E38F-4A22-A369-7B516850B6CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A820D6-A2DD-4D4C-A355-56BF217EAE65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de prueba" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="287">
   <si>
     <t>PASOS</t>
   </si>
@@ -1373,6 +1373,111 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1400,112 +1505,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1526,14 +1529,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3618,6 +3618,159 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>647090</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>433730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75674461-C936-4FF7-B548-25AE8950D143}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18539460" y="487680"/>
+          <a:ext cx="288950" cy="288950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>654710</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>487070</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C0C3B6A-62F8-4E35-9EB5-C8DF7A193997}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18547080" y="1211580"/>
+          <a:ext cx="288950" cy="288950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>662330</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>502310</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E8EF50-4D14-44EC-9E84-8E8A1B4EF739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18554700" y="1897380"/>
+          <a:ext cx="288950" cy="288950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3847,24 +4000,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="31.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="62" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="51" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="62"/>
     </row>
     <row r="2" spans="1:19" ht="27" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3905,19 +4058,19 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="52" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="46">
         <v>1</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="46" t="s">
         <v>96</v>
       </c>
       <c r="F3" s="7">
@@ -3929,23 +4082,23 @@
       <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="54">
+      <c r="K3" s="63">
         <v>44869</v>
       </c>
-      <c r="L3" s="54"/>
+      <c r="L3" s="63"/>
     </row>
     <row r="4" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="49"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="7">
         <v>2</v>
       </c>
@@ -3955,25 +4108,25 @@
       <c r="H4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="52" t="s">
         <v>269</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="46">
         <v>1</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="7">
@@ -3985,23 +4138,23 @@
       <c r="H5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="56">
+      <c r="K5" s="65">
         <v>44869</v>
       </c>
-      <c r="L5" s="56"/>
+      <c r="L5" s="65"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="49"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="7">
         <v>2</v>
       </c>
@@ -4011,17 +4164,17 @@
       <c r="H6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="49"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="7">
         <v>3</v>
       </c>
@@ -4031,17 +4184,17 @@
       <c r="H7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
     </row>
     <row r="8" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="49"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="7">
         <v>4</v>
       </c>
@@ -4051,25 +4204,25 @@
       <c r="H8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="47"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="46">
         <v>1</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="46" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="8">
@@ -4081,16 +4234,16 @@
       <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K9" s="50">
+      <c r="K9" s="51">
         <v>44869</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="51"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -4100,11 +4253,11 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="49"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="8">
         <v>2</v>
       </c>
@@ -4114,10 +4267,10 @@
       <c r="H10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -4127,11 +4280,11 @@
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="49"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="8">
         <v>3</v>
       </c>
@@ -4141,10 +4294,10 @@
       <c r="H11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
       <c r="M11"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -4154,11 +4307,11 @@
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="49"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="8">
         <v>4</v>
       </c>
@@ -4168,10 +4321,10 @@
       <c r="H12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -4217,19 +4370,19 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="74" t="s">
         <v>272</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="71">
         <v>1</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="74" t="s">
         <v>255</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="74" t="s">
         <v>256</v>
       </c>
       <c r="F14" s="8">
@@ -4244,20 +4397,20 @@
       <c r="I14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="68">
         <v>44869</v>
       </c>
-      <c r="L14" s="33"/>
+      <c r="L14" s="68"/>
     </row>
     <row r="15" spans="1:19" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
       <c r="F15" s="8">
         <v>2</v>
       </c>
@@ -4270,16 +4423,16 @@
       <c r="I15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
     </row>
     <row r="16" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
       <c r="F16" s="8">
         <v>3</v>
       </c>
@@ -4292,16 +4445,16 @@
       <c r="I16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
     </row>
     <row r="17" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="8">
         <v>4</v>
       </c>
@@ -4314,24 +4467,24 @@
       <c r="I17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
     </row>
     <row r="18" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="74" t="s">
         <v>273</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="71">
         <v>1</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="74" t="s">
         <v>256</v>
       </c>
       <c r="F18" s="8">
@@ -4346,20 +4499,20 @@
       <c r="I18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="36" t="s">
+      <c r="J18" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="33">
+      <c r="K18" s="68">
         <v>44869</v>
       </c>
-      <c r="L18" s="33"/>
+      <c r="L18" s="68"/>
     </row>
     <row r="19" spans="1:12" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
       <c r="F19" s="8">
         <v>2</v>
       </c>
@@ -4372,16 +4525,16 @@
       <c r="I19" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
     </row>
     <row r="20" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
       <c r="F20" s="8">
         <v>3</v>
       </c>
@@ -4394,16 +4547,16 @@
       <c r="I20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
     </row>
     <row r="21" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
       <c r="F21" s="8">
         <v>4</v>
       </c>
@@ -4416,24 +4569,24 @@
       <c r="I21" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="38"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
     </row>
     <row r="22" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="46">
         <v>1</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="46" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="8">
@@ -4448,20 +4601,20 @@
       <c r="I22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="48" t="s">
+      <c r="J22" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K22" s="50">
+      <c r="K22" s="51">
         <v>44869</v>
       </c>
-      <c r="L22" s="50"/>
+      <c r="L22" s="51"/>
     </row>
     <row r="23" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="49"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="8">
         <v>2</v>
       </c>
@@ -4474,16 +4627,16 @@
       <c r="I23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
     </row>
     <row r="24" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="49"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="8">
         <v>3</v>
       </c>
@@ -4496,24 +4649,24 @@
       <c r="I24" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
     </row>
     <row r="25" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="45" t="s">
         <v>275</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="46">
         <v>1</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="46" t="s">
         <v>35</v>
       </c>
       <c r="F25" s="8">
@@ -4528,20 +4681,20 @@
       <c r="I25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="48" t="s">
+      <c r="J25" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K25" s="50">
+      <c r="K25" s="51">
         <v>44869</v>
       </c>
-      <c r="L25" s="50"/>
+      <c r="L25" s="51"/>
     </row>
     <row r="26" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="8">
         <v>2</v>
       </c>
@@ -4554,16 +4707,16 @@
       <c r="I26" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
     </row>
     <row r="27" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="49"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="8">
         <v>3</v>
       </c>
@@ -4576,24 +4729,24 @@
       <c r="I27" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
     </row>
     <row r="28" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="46">
         <v>1</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="46" t="s">
         <v>39</v>
       </c>
       <c r="F28" s="8">
@@ -4608,20 +4761,20 @@
       <c r="I28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="48" t="s">
+      <c r="J28" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K28" s="50">
+      <c r="K28" s="51">
         <v>44869</v>
       </c>
-      <c r="L28" s="50"/>
+      <c r="L28" s="51"/>
     </row>
     <row r="29" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="49"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="8">
         <v>2</v>
       </c>
@@ -4634,16 +4787,16 @@
       <c r="I29" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
     </row>
     <row r="30" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="49"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="8">
         <v>3</v>
       </c>
@@ -4656,9 +4809,9 @@
       <c r="I30" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
     </row>
     <row r="31" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
@@ -4697,19 +4850,19 @@
       <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="46">
         <v>1</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="46" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="8">
@@ -4721,23 +4874,23 @@
       <c r="H32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="46" t="s">
+      <c r="I32" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="48" t="s">
+      <c r="J32" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K32" s="50">
+      <c r="K32" s="51">
         <v>44869</v>
       </c>
-      <c r="L32" s="50"/>
+      <c r="L32" s="51"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="49"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="47"/>
       <c r="F33" s="8">
         <v>2</v>
       </c>
@@ -4747,17 +4900,17 @@
       <c r="H33" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="47"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="49"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="47"/>
       <c r="F34" s="8">
         <v>3</v>
       </c>
@@ -4767,17 +4920,17 @@
       <c r="H34" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I34" s="47"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="49"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="8">
         <v>4</v>
       </c>
@@ -4787,17 +4940,17 @@
       <c r="H35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="47"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="49"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="47"/>
       <c r="F36" s="8">
         <v>5</v>
       </c>
@@ -4807,17 +4960,17 @@
       <c r="H36" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="I36" s="47"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="49"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="47"/>
       <c r="F37" s="8">
         <v>6</v>
       </c>
@@ -4827,17 +4980,17 @@
       <c r="H37" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I37" s="47"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="49"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="8">
         <v>7</v>
       </c>
@@ -4847,17 +5000,17 @@
       <c r="H38" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I38" s="47"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="49"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="47"/>
       <c r="F39" s="8">
         <v>8</v>
       </c>
@@ -4867,25 +5020,25 @@
       <c r="H39" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I39" s="47"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C40" s="46">
         <v>1</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="E40" s="48" t="s">
+      <c r="E40" s="46" t="s">
         <v>56</v>
       </c>
       <c r="F40" s="8">
@@ -4897,23 +5050,23 @@
       <c r="H40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I40" s="46" t="s">
+      <c r="I40" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="48" t="s">
+      <c r="J40" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K40" s="50">
+      <c r="K40" s="51">
         <v>44869</v>
       </c>
-      <c r="L40" s="50"/>
+      <c r="L40" s="51"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="49"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="8">
         <v>2</v>
       </c>
@@ -4923,17 +5076,17 @@
       <c r="H41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I41" s="47"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="49"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="8">
         <v>3</v>
       </c>
@@ -4943,17 +5096,17 @@
       <c r="H42" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I42" s="47"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
     </row>
     <row r="43" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="49"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="8">
         <v>4</v>
       </c>
@@ -4963,17 +5116,17 @@
       <c r="H43" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I43" s="47"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="49"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="47"/>
       <c r="F44" s="8">
         <v>5</v>
       </c>
@@ -4983,17 +5136,17 @@
       <c r="H44" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="47"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
     </row>
     <row r="45" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="49"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="8">
         <v>6</v>
       </c>
@@ -5003,25 +5156,25 @@
       <c r="H45" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I45" s="47"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="59" t="s">
+      <c r="A46" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="48">
+      <c r="C46" s="46">
         <v>1</v>
       </c>
-      <c r="D46" s="48" t="s">
+      <c r="D46" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="46" t="s">
         <v>71</v>
       </c>
       <c r="F46" s="8">
@@ -5033,23 +5186,23 @@
       <c r="H46" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I46" s="46" t="s">
+      <c r="I46" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J46" s="48" t="s">
+      <c r="J46" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K46" s="50">
+      <c r="K46" s="51">
         <v>44869</v>
       </c>
-      <c r="L46" s="50"/>
+      <c r="L46" s="51"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="49"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="8">
         <v>2</v>
       </c>
@@ -5059,17 +5212,17 @@
       <c r="H47" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I47" s="47"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
     </row>
     <row r="48" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="49"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="8">
         <v>3</v>
       </c>
@@ -5079,10 +5232,10 @@
       <c r="H48" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="I48" s="47"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
     </row>
     <row r="49" spans="1:16384" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
@@ -5193,19 +5346,19 @@
       <c r="L51" s="11"/>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="48" t="s">
+      <c r="B52" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="48">
+      <c r="C52" s="46">
         <v>1</v>
       </c>
-      <c r="D52" s="48" t="s">
+      <c r="D52" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="48" t="s">
+      <c r="E52" s="46" t="s">
         <v>283</v>
       </c>
       <c r="F52" s="8">
@@ -5217,23 +5370,23 @@
       <c r="H52" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I52" s="46" t="s">
+      <c r="I52" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="48" t="s">
+      <c r="J52" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="K52" s="50">
+      <c r="K52" s="51">
         <v>44869</v>
       </c>
-      <c r="L52" s="50"/>
+      <c r="L52" s="51"/>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="49"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="47"/>
       <c r="F53" s="8">
         <v>2</v>
       </c>
@@ -5243,17 +5396,17 @@
       <c r="H53" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="I53" s="47"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47"/>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="49"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="8">
         <v>3</v>
       </c>
@@ -5263,17 +5416,17 @@
       <c r="H54" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I54" s="47"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="47"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="47"/>
     </row>
     <row r="55" spans="1:16384" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A55" s="49"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="49"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="8">
         <v>4</v>
       </c>
@@ -5283,25 +5436,25 @@
       <c r="H55" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="I55" s="47"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="49"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
     </row>
     <row r="56" spans="1:16384" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="38">
         <v>2</v>
       </c>
-      <c r="D56" s="43" t="s">
+      <c r="D56" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="38" t="s">
         <v>163</v>
       </c>
       <c r="F56" s="22">
@@ -5316,18 +5469,18 @@
       <c r="I56" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J56" s="59" t="s">
+      <c r="J56" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38"/>
     </row>
     <row r="57" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
       <c r="F57" s="22">
         <v>2</v>
       </c>
@@ -5340,16 +5493,16 @@
       <c r="I57" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="48"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="43"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
     </row>
     <row r="58" spans="1:16384" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
       <c r="F58" s="29">
         <v>3</v>
       </c>
@@ -5362,24 +5515,24 @@
       <c r="I58" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="J58" s="48"/>
-      <c r="K58" s="43"/>
-      <c r="L58" s="43"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="38"/>
+      <c r="L58" s="38"/>
     </row>
     <row r="59" spans="1:16384" s="22" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="68" t="s">
+      <c r="A59" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="B59" s="71" t="s">
+      <c r="B59" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="71">
+      <c r="C59" s="42">
         <v>2</v>
       </c>
-      <c r="D59" s="71" t="s">
+      <c r="D59" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="39" t="s">
         <v>174</v>
       </c>
       <c r="F59" s="22">
@@ -5394,11 +5547,11 @@
       <c r="I59" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J59" s="68" t="s">
+      <c r="J59" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="K59" s="71"/>
-      <c r="L59" s="71"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -21773,11 +21926,11 @@
       <c r="XFD59" s="4"/>
     </row>
     <row r="60" spans="1:16384" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A60" s="72"/>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
       <c r="F60" s="22">
         <v>2</v>
       </c>
@@ -21790,9 +21943,9 @@
       <c r="I60" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J60" s="69"/>
-      <c r="K60" s="72"/>
-      <c r="L60" s="72"/>
+      <c r="J60" s="40"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -38167,11 +38320,11 @@
       <c r="XFD60" s="4"/>
     </row>
     <row r="61" spans="1:16384" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A61" s="72"/>
-      <c r="B61" s="72"/>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
       <c r="F61" s="22">
         <v>3</v>
       </c>
@@ -38184,9 +38337,9 @@
       <c r="I61" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J61" s="69"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="43"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -54561,11 +54714,11 @@
       <c r="XFD61" s="4"/>
     </row>
     <row r="62" spans="1:16384" s="22" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A62" s="73"/>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
       <c r="F62" s="22">
         <v>4</v>
       </c>
@@ -54578,9 +54731,9 @@
       <c r="I62" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J62" s="70"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="73"/>
+      <c r="J62" s="41"/>
+      <c r="K62" s="44"/>
+      <c r="L62" s="44"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -70955,19 +71108,19 @@
       <c r="XFD62" s="4"/>
     </row>
     <row r="63" spans="1:16384" s="18" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="42" t="s">
+      <c r="A63" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="38">
         <v>2</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="E63" s="42" t="s">
+      <c r="E63" s="37" t="s">
         <v>174</v>
       </c>
       <c r="F63" s="22">
@@ -70982,18 +71135,18 @@
       <c r="I63" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J63" s="42" t="s">
+      <c r="J63" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="K63" s="43"/>
-      <c r="L63" s="43"/>
+      <c r="K63" s="38"/>
+      <c r="L63" s="38"/>
     </row>
     <row r="64" spans="1:16384" s="18" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A64" s="42"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
       <c r="F64" s="22">
         <v>2</v>
       </c>
@@ -71006,16 +71159,16 @@
       <c r="I64" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J64" s="42"/>
-      <c r="K64" s="43"/>
-      <c r="L64" s="43"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
     </row>
     <row r="65" spans="1:12" s="18" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
       <c r="F65" s="22">
         <v>3</v>
       </c>
@@ -71028,24 +71181,24 @@
       <c r="I65" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="J65" s="42"/>
-      <c r="K65" s="43"/>
-      <c r="L65" s="43"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
     </row>
     <row r="66" spans="1:12" s="18" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="s">
+      <c r="A66" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="38">
         <v>2</v>
       </c>
-      <c r="D66" s="42" t="s">
+      <c r="D66" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="E66" s="42" t="s">
+      <c r="E66" s="37" t="s">
         <v>201</v>
       </c>
       <c r="F66" s="27">
@@ -71054,68 +71207,68 @@
       <c r="G66" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="H66" s="42" t="s">
+      <c r="H66" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="I66" s="43" t="s">
+      <c r="I66" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J66" s="43" t="s">
+      <c r="J66" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K66" s="43"/>
-      <c r="L66" s="43"/>
+      <c r="K66" s="38"/>
+      <c r="L66" s="38"/>
     </row>
     <row r="67" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
-      <c r="B67" s="42"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="43"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="38"/>
       <c r="F67" s="31">
         <v>2</v>
       </c>
       <c r="G67" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
-      <c r="J67" s="43"/>
-      <c r="K67" s="43"/>
-      <c r="L67" s="43"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
     </row>
     <row r="68" spans="1:12" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A68" s="42"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="43"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="38"/>
       <c r="F68" s="31">
         <v>3</v>
       </c>
       <c r="G68" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
-      <c r="J68" s="43"/>
-      <c r="K68" s="43"/>
-      <c r="L68" s="43"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
+      <c r="L68" s="38"/>
     </row>
     <row r="69" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A69" s="42" t="s">
+      <c r="A69" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="C69" s="43">
+      <c r="C69" s="38">
         <v>2</v>
       </c>
-      <c r="D69" s="42" t="s">
+      <c r="D69" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="E69" s="42" t="s">
+      <c r="E69" s="37" t="s">
         <v>206</v>
       </c>
       <c r="F69" s="27">
@@ -71124,68 +71277,68 @@
       <c r="G69" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="H69" s="42" t="s">
+      <c r="H69" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="I69" s="43" t="s">
+      <c r="I69" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J69" s="43" t="s">
+      <c r="J69" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K69" s="45"/>
-      <c r="L69" s="45"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="43"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="38"/>
       <c r="F70" s="31">
         <v>2</v>
       </c>
       <c r="G70" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="43"/>
-      <c r="K70" s="45"/>
-      <c r="L70" s="45"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="36"/>
     </row>
     <row r="71" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A71" s="42"/>
-      <c r="B71" s="42"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="43"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="38"/>
       <c r="F71" s="31">
         <v>3</v>
       </c>
       <c r="G71" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="43"/>
-      <c r="K71" s="45"/>
-      <c r="L71" s="45"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="36"/>
+      <c r="L71" s="36"/>
     </row>
     <row r="72" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A72" s="42" t="s">
+      <c r="A72" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C72" s="43">
+      <c r="C72" s="38">
         <v>2</v>
       </c>
-      <c r="D72" s="42" t="s">
+      <c r="D72" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="E72" s="42" t="s">
+      <c r="E72" s="37" t="s">
         <v>163</v>
       </c>
       <c r="F72" s="27">
@@ -71194,68 +71347,68 @@
       <c r="G72" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="H72" s="42" t="s">
+      <c r="H72" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="I72" s="43" t="s">
+      <c r="I72" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J72" s="43" t="s">
+      <c r="J72" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K72" s="45"/>
-      <c r="L72" s="45"/>
+      <c r="K72" s="36"/>
+      <c r="L72" s="36"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="42"/>
-      <c r="B73" s="42"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="43"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="38"/>
       <c r="F73" s="31">
         <v>2</v>
       </c>
       <c r="G73" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="45"/>
-      <c r="L73" s="45"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="36"/>
+      <c r="L73" s="36"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="42"/>
-      <c r="B74" s="42"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="43"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="38"/>
       <c r="F74" s="31">
         <v>3</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="H74" s="43"/>
-      <c r="I74" s="43"/>
-      <c r="J74" s="43"/>
-      <c r="K74" s="45"/>
-      <c r="L74" s="45"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
     </row>
     <row r="75" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A75" s="42" t="s">
+      <c r="A75" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="43">
+      <c r="C75" s="38">
         <v>2</v>
       </c>
-      <c r="D75" s="42" t="s">
+      <c r="D75" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="E75" s="42" t="s">
+      <c r="E75" s="37" t="s">
         <v>163</v>
       </c>
       <c r="F75" s="27">
@@ -71264,68 +71417,68 @@
       <c r="G75" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="H75" s="42" t="s">
+      <c r="H75" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="I75" s="43" t="s">
+      <c r="I75" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J75" s="43" t="s">
+      <c r="J75" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K75" s="45"/>
-      <c r="L75" s="45"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="42"/>
-      <c r="B76" s="42"/>
-      <c r="C76" s="43"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="43"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="38"/>
       <c r="F76" s="31">
         <v>2</v>
       </c>
       <c r="G76" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="45"/>
-      <c r="L76" s="45"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+      <c r="J76" s="38"/>
+      <c r="K76" s="36"/>
+      <c r="L76" s="36"/>
     </row>
     <row r="77" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A77" s="42"/>
-      <c r="B77" s="42"/>
-      <c r="C77" s="43"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="43"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="38"/>
       <c r="F77" s="31">
         <v>3</v>
       </c>
       <c r="G77" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="45"/>
-      <c r="L77" s="45"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="36"/>
     </row>
     <row r="78" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A78" s="42" t="s">
+      <c r="A78" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="B78" s="42" t="s">
+      <c r="B78" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="C78" s="43">
+      <c r="C78" s="38">
         <v>2</v>
       </c>
-      <c r="D78" s="42" t="s">
+      <c r="D78" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="E78" s="42" t="s">
+      <c r="E78" s="37" t="s">
         <v>163</v>
       </c>
       <c r="F78" s="27">
@@ -71334,68 +71487,68 @@
       <c r="G78" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="H78" s="42" t="s">
+      <c r="H78" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="I78" s="43" t="s">
+      <c r="I78" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J78" s="43" t="s">
+      <c r="J78" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K78" s="45"/>
-      <c r="L78" s="45"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="36"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="42"/>
-      <c r="B79" s="42"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="43"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="38"/>
       <c r="F79" s="31">
         <v>2</v>
       </c>
       <c r="G79" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="45"/>
-      <c r="L79" s="45"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="36"/>
+      <c r="L79" s="36"/>
     </row>
     <row r="80" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A80" s="42"/>
-      <c r="B80" s="42"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="43"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="38"/>
       <c r="F80" s="31">
         <v>3</v>
       </c>
       <c r="G80" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="H80" s="43"/>
-      <c r="I80" s="43"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="45"/>
-      <c r="L80" s="45"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="36"/>
+      <c r="L80" s="36"/>
     </row>
     <row r="81" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A81" s="42" t="s">
+      <c r="A81" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="C81" s="43">
+      <c r="C81" s="38">
         <v>2</v>
       </c>
-      <c r="D81" s="42" t="s">
+      <c r="D81" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="E81" s="42" t="s">
+      <c r="E81" s="37" t="s">
         <v>163</v>
       </c>
       <c r="F81" s="27">
@@ -71404,68 +71557,68 @@
       <c r="G81" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="H81" s="42" t="s">
+      <c r="H81" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="I81" s="43" t="s">
+      <c r="I81" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J81" s="43" t="s">
+      <c r="J81" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K81" s="45"/>
-      <c r="L81" s="45"/>
+      <c r="K81" s="36"/>
+      <c r="L81" s="36"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="42"/>
-      <c r="B82" s="42"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="43"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="38"/>
       <c r="F82" s="31">
         <v>2</v>
       </c>
       <c r="G82" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="H82" s="43"/>
-      <c r="I82" s="43"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="45"/>
-      <c r="L82" s="45"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
+      <c r="J82" s="38"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="36"/>
     </row>
     <row r="83" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A83" s="42"/>
-      <c r="B83" s="42"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="43"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="38"/>
       <c r="F83" s="31">
         <v>3</v>
       </c>
       <c r="G83" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="45"/>
-      <c r="L83" s="45"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="38"/>
+      <c r="J83" s="38"/>
+      <c r="K83" s="36"/>
+      <c r="L83" s="36"/>
     </row>
     <row r="84" spans="1:12" s="5" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="44" t="s">
+      <c r="A84" s="67" t="s">
         <v>278</v>
       </c>
-      <c r="B84" s="42" t="s">
+      <c r="B84" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="45">
+      <c r="C84" s="36">
         <v>2</v>
       </c>
-      <c r="D84" s="42" t="s">
+      <c r="D84" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="E84" s="44" t="s">
+      <c r="E84" s="67" t="s">
         <v>174</v>
       </c>
       <c r="F84" s="31">
@@ -71474,68 +71627,187 @@
       <c r="G84" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="H84" s="42" t="s">
+      <c r="H84" s="37" t="s">
         <v>238</v>
       </c>
       <c r="I84" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="J84" s="44" t="s">
+      <c r="J84" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="K84" s="45"/>
-      <c r="L84" s="45"/>
+      <c r="K84" s="36"/>
+      <c r="L84" s="36"/>
     </row>
     <row r="85" spans="1:12" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A85" s="44"/>
-      <c r="B85" s="42"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="44"/>
+      <c r="A85" s="67"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="67"/>
       <c r="F85" s="31">
         <v>2</v>
       </c>
       <c r="G85" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H85" s="43"/>
+      <c r="H85" s="38"/>
       <c r="I85" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="J85" s="45"/>
-      <c r="K85" s="45"/>
-      <c r="L85" s="45"/>
+      <c r="J85" s="36"/>
+      <c r="K85" s="36"/>
+      <c r="L85" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="199">
-    <mergeCell ref="K84:K85"/>
-    <mergeCell ref="L84:L85"/>
-    <mergeCell ref="L69:L71"/>
-    <mergeCell ref="K69:K71"/>
-    <mergeCell ref="K72:K74"/>
-    <mergeCell ref="L72:L74"/>
-    <mergeCell ref="K75:K77"/>
-    <mergeCell ref="L75:L77"/>
-    <mergeCell ref="K78:K80"/>
-    <mergeCell ref="L78:L80"/>
-    <mergeCell ref="K81:K83"/>
-    <mergeCell ref="L81:L83"/>
-    <mergeCell ref="J63:J65"/>
-    <mergeCell ref="L63:L65"/>
-    <mergeCell ref="K63:K65"/>
-    <mergeCell ref="E63:E65"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="J59:J62"/>
-    <mergeCell ref="K59:K62"/>
-    <mergeCell ref="L59:L62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="H81:H83"/>
+    <mergeCell ref="I81:I83"/>
+    <mergeCell ref="J81:J83"/>
+    <mergeCell ref="H84:H85"/>
+    <mergeCell ref="J84:J85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="H75:H77"/>
+    <mergeCell ref="I75:I77"/>
+    <mergeCell ref="J75:J77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="H78:H80"/>
+    <mergeCell ref="I78:I80"/>
+    <mergeCell ref="J78:J80"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="E69:E71"/>
+    <mergeCell ref="H69:H71"/>
+    <mergeCell ref="I69:I71"/>
+    <mergeCell ref="J69:J71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="H72:H74"/>
+    <mergeCell ref="I72:I74"/>
+    <mergeCell ref="J72:J74"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="H66:H68"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="I66:I68"/>
+    <mergeCell ref="J66:J68"/>
+    <mergeCell ref="L66:L68"/>
+    <mergeCell ref="K66:K68"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="K46:K48"/>
+    <mergeCell ref="L52:L55"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="L32:L39"/>
+    <mergeCell ref="L40:L45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J5:J8"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="C40:C45"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="I5:I8"/>
     <mergeCell ref="E56:E58"/>
     <mergeCell ref="D56:D58"/>
     <mergeCell ref="C56:C58"/>
@@ -71560,153 +71832,34 @@
     <mergeCell ref="K40:K45"/>
     <mergeCell ref="C32:C39"/>
     <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="J5:J8"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="K46:K48"/>
-    <mergeCell ref="L52:L55"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="L32:L39"/>
-    <mergeCell ref="L40:L45"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="H66:H68"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="I66:I68"/>
-    <mergeCell ref="J66:J68"/>
-    <mergeCell ref="L66:L68"/>
-    <mergeCell ref="K66:K68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="H69:H71"/>
-    <mergeCell ref="I69:I71"/>
-    <mergeCell ref="J69:J71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="E72:E74"/>
-    <mergeCell ref="H72:H74"/>
-    <mergeCell ref="I72:I74"/>
-    <mergeCell ref="J72:J74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="H75:H77"/>
-    <mergeCell ref="I75:I77"/>
-    <mergeCell ref="J75:J77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="H78:H80"/>
-    <mergeCell ref="I78:I80"/>
-    <mergeCell ref="J78:J80"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="H81:H83"/>
-    <mergeCell ref="I81:I83"/>
-    <mergeCell ref="J81:J83"/>
-    <mergeCell ref="H84:H85"/>
-    <mergeCell ref="J84:J85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="J63:J65"/>
+    <mergeCell ref="L63:L65"/>
+    <mergeCell ref="K63:K65"/>
+    <mergeCell ref="E63:E65"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="J59:J62"/>
+    <mergeCell ref="K59:K62"/>
+    <mergeCell ref="L59:L62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="K84:K85"/>
+    <mergeCell ref="L84:L85"/>
+    <mergeCell ref="L69:L71"/>
+    <mergeCell ref="K69:K71"/>
+    <mergeCell ref="K72:K74"/>
+    <mergeCell ref="L72:L74"/>
+    <mergeCell ref="K75:K77"/>
+    <mergeCell ref="L75:L77"/>
+    <mergeCell ref="K78:K80"/>
+    <mergeCell ref="L78:L80"/>
+    <mergeCell ref="K81:K83"/>
+    <mergeCell ref="L81:L83"/>
   </mergeCells>
   <conditionalFormatting sqref="I3:I13 I84:I1048576 I22:I66">
     <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
@@ -71860,8 +72013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51632221-CBA9-4331-99E3-692DAE49CE90}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -71886,80 +72039,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" customFormat="1" ht="13.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="H1" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="79"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="74" t="s">
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="O1" s="74" t="s">
+      <c r="O1" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="74" t="s">
+      <c r="P1" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="74" t="s">
+      <c r="Q1" s="77" t="s">
         <v>242</v>
       </c>
-      <c r="R1" s="74" t="s">
+      <c r="R1" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="S1" s="74" t="s">
+      <c r="S1" s="77" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="75"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:19" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -71983,11 +72136,11 @@
       <c r="G3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="22" t="s">
         <v>159</v>
       </c>
@@ -72034,11 +72187,11 @@
       <c r="G4" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="22" t="s">
         <v>159</v>
       </c>
@@ -72085,11 +72238,11 @@
       <c r="G5" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="22" t="s">
         <v>159</v>
       </c>
@@ -72116,11 +72269,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
@@ -72130,12 +72284,11 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="H1:J2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K1048576">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
@@ -72179,7 +72332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3781BE-730A-4157-B2E2-6982EC8E895A}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -72201,57 +72354,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="77" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="77" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="75"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="78"/>
     </row>
     <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="84">
+      <c r="A3" s="33">
         <v>44869</v>
       </c>
-      <c r="B3" s="85">
+      <c r="B3" s="34">
         <v>1</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="34" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="32" t="s">
@@ -72277,13 +72430,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="84">
+      <c r="A4" s="33">
         <v>44869</v>
       </c>
-      <c r="B4" s="85">
+      <c r="B4" s="34">
         <v>1</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="34" t="s">
         <v>112</v>
       </c>
       <c r="D4" s="32" t="s">
@@ -72309,13 +72462,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="84">
+      <c r="A5" s="33">
         <v>44869</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="34">
         <v>1</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="34" t="s">
         <v>113</v>
       </c>
       <c r="D5" s="32" t="s">
@@ -72341,13 +72494,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="84">
+      <c r="A6" s="33">
         <v>44869</v>
       </c>
-      <c r="B6" s="85">
+      <c r="B6" s="34">
         <v>1</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="34" t="s">
         <v>114</v>
       </c>
       <c r="D6" s="32" t="s">
@@ -72373,13 +72526,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="84">
+      <c r="A7" s="33">
         <v>44869</v>
       </c>
-      <c r="B7" s="85">
+      <c r="B7" s="34">
         <v>1</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="34" t="s">
         <v>115</v>
       </c>
       <c r="D7" s="32" t="s">
@@ -72405,13 +72558,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="84">
+      <c r="A8" s="33">
         <v>44869</v>
       </c>
-      <c r="B8" s="85">
+      <c r="B8" s="34">
         <v>1</v>
       </c>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="34" t="s">
         <v>116</v>
       </c>
       <c r="D8" s="32" t="s">
@@ -72437,13 +72590,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="84">
+      <c r="A9" s="33">
         <v>44869</v>
       </c>
-      <c r="B9" s="85">
+      <c r="B9" s="34">
         <v>1</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="34" t="s">
         <v>117</v>
       </c>
       <c r="D9" s="32" t="s">
@@ -72455,13 +72608,13 @@
       <c r="F9" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="84">
+      <c r="G9" s="33">
         <v>44869</v>
       </c>
       <c r="H9" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="I9" s="84">
+      <c r="I9" s="33">
         <v>44871</v>
       </c>
       <c r="J9" s="32" t="s">
@@ -72469,13 +72622,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="84">
+      <c r="A10" s="33">
         <v>44869</v>
       </c>
-      <c r="B10" s="85">
+      <c r="B10" s="34">
         <v>1</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="34" t="s">
         <v>118</v>
       </c>
       <c r="D10" s="32" t="s">
@@ -72487,13 +72640,13 @@
       <c r="F10" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="84">
+      <c r="G10" s="33">
         <v>44869</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="I10" s="84">
+      <c r="I10" s="33">
         <v>44871</v>
       </c>
       <c r="J10" s="32" t="s">
@@ -72501,13 +72654,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="84">
+      <c r="A11" s="33">
         <v>44869</v>
       </c>
-      <c r="B11" s="85">
+      <c r="B11" s="34">
         <v>1</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="34" t="s">
         <v>119</v>
       </c>
       <c r="D11" s="32" t="s">
@@ -72519,13 +72672,13 @@
       <c r="F11" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="G11" s="84">
+      <c r="G11" s="33">
         <v>44869</v>
       </c>
       <c r="H11" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="I11" s="84">
+      <c r="I11" s="33">
         <v>44871</v>
       </c>
       <c r="J11" s="32" t="s">
@@ -72533,13 +72686,13 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="84">
+      <c r="A12" s="33">
         <v>44869</v>
       </c>
-      <c r="B12" s="85">
+      <c r="B12" s="34">
         <v>1</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="34" t="s">
         <v>120</v>
       </c>
       <c r="D12" s="32" t="s">
@@ -72565,13 +72718,13 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="84">
+      <c r="A13" s="33">
         <v>44869</v>
       </c>
-      <c r="B13" s="85">
+      <c r="B13" s="34">
         <v>1</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="34" t="s">
         <v>121</v>
       </c>
       <c r="D13" s="32" t="s">
@@ -72597,13 +72750,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="84">
+      <c r="A14" s="33">
         <v>44869</v>
       </c>
-      <c r="B14" s="85">
+      <c r="B14" s="34">
         <v>1</v>
       </c>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="34" t="s">
         <v>122</v>
       </c>
       <c r="D14" s="32" t="s">
@@ -72629,13 +72782,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="84">
+      <c r="A15" s="33">
         <v>44869</v>
       </c>
-      <c r="B15" s="85">
+      <c r="B15" s="34">
         <v>1</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="34" t="s">
         <v>123</v>
       </c>
       <c r="D15" s="32" t="s">
@@ -72661,13 +72814,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="84">
+      <c r="A16" s="33">
         <v>44869</v>
       </c>
-      <c r="B16" s="85">
+      <c r="B16" s="34">
         <v>1</v>
       </c>
-      <c r="C16" s="85" t="s">
+      <c r="C16" s="34" t="s">
         <v>124</v>
       </c>
       <c r="D16" s="32" t="s">
@@ -72693,13 +72846,13 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="84">
+      <c r="A17" s="33">
         <v>44869</v>
       </c>
-      <c r="B17" s="85">
+      <c r="B17" s="34">
         <v>1</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="34" t="s">
         <v>125</v>
       </c>
       <c r="D17" s="32" t="s">
@@ -72725,13 +72878,13 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="84">
+      <c r="A18" s="33">
         <v>44869</v>
       </c>
-      <c r="B18" s="85">
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="85" t="s">
+      <c r="C18" s="34" t="s">
         <v>160</v>
       </c>
       <c r="D18" s="32" t="s">
@@ -72757,13 +72910,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="84">
+      <c r="A19" s="33">
         <v>44869</v>
       </c>
-      <c r="B19" s="85">
+      <c r="B19" s="34">
         <v>1</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="34" t="s">
         <v>171</v>
       </c>
       <c r="D19" s="32" t="s">
@@ -72792,10 +72945,10 @@
       <c r="A20" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="86">
+      <c r="B20" s="35">
         <v>2</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="35" t="s">
         <v>190</v>
       </c>
       <c r="D20" s="32" t="s">
@@ -72824,10 +72977,10 @@
       <c r="A21" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="86">
+      <c r="B21" s="35">
         <v>2</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="35" t="s">
         <v>196</v>
       </c>
       <c r="D21" s="32" t="s">
@@ -72856,10 +73009,10 @@
       <c r="A22" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="86">
+      <c r="B22" s="35">
         <v>2</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="35" t="s">
         <v>202</v>
       </c>
       <c r="D22" s="32" t="s">
@@ -72888,10 +73041,10 @@
       <c r="A23" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B23" s="86">
+      <c r="B23" s="35">
         <v>2</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="35" t="s">
         <v>208</v>
       </c>
       <c r="D23" s="32" t="s">
@@ -72920,10 +73073,10 @@
       <c r="A24" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B24" s="86">
+      <c r="B24" s="35">
         <v>2</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="35" t="s">
         <v>214</v>
       </c>
       <c r="D24" s="32" t="s">
@@ -72952,10 +73105,10 @@
       <c r="A25" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B25" s="86">
+      <c r="B25" s="35">
         <v>2</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="35" t="s">
         <v>221</v>
       </c>
       <c r="D25" s="32" t="s">
@@ -72984,10 +73137,10 @@
       <c r="A26" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B26" s="86">
+      <c r="B26" s="35">
         <v>2</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="35" t="s">
         <v>226</v>
       </c>
       <c r="D26" s="32" t="s">
@@ -73016,10 +73169,10 @@
       <c r="A27" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B27" s="86">
+      <c r="B27" s="35">
         <v>2</v>
       </c>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="35" t="s">
         <v>233</v>
       </c>
       <c r="D27" s="32" t="s">
@@ -73048,10 +73201,10 @@
       <c r="A28" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B28" s="86">
+      <c r="B28" s="35">
         <v>2</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="35" t="s">
         <v>277</v>
       </c>
       <c r="D28" s="32" t="s">
@@ -73080,10 +73233,10 @@
       <c r="A29" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B29" s="86">
+      <c r="B29" s="35">
         <v>2</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="35" t="s">
         <v>278</v>
       </c>
       <c r="D29" s="32" t="s">
@@ -73110,16 +73263,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">

</xml_diff>